<commit_message>
Updated Results with corrected code
</commit_message>
<xml_diff>
--- a/Scripts/Industry/Results_per_Country/2030_AT.xlsx
+++ b/Scripts/Industry/Results_per_Country/2030_AT.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,12 +467,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1610397.083213597</v>
+        <v>1625037.056697357</v>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
-        <v>215.3785089235195</v>
-      </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -482,7 +480,7 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
-        <v>18717.51968611433</v>
+        <v>33.93168714694506</v>
       </c>
       <c r="D4" t="inlineStr"/>
     </row>
@@ -494,7 +492,7 @@
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
-        <v>76403.23314026152</v>
+        <v>2424.883513345702</v>
       </c>
       <c r="D5" t="inlineStr"/>
     </row>
@@ -513,13 +511,25 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Biogas</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>269.0658853011937</v>
+        <v>411.770166210904</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>126.8499407842672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update results for Steel
</commit_message>
<xml_diff>
--- a/Scripts/Industry/Results_per_Country/2030_AT.xlsx
+++ b/Scripts/Industry/Results_per_Country/2030_AT.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1625037.056697357</v>
+        <v>1465.462811187185</v>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
@@ -480,7 +480,7 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
-        <v>33.93168714694506</v>
+        <v>33.93168714694505</v>
       </c>
       <c r="D4" t="inlineStr"/>
     </row>
@@ -492,7 +492,7 @@
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
-        <v>2424.883513345702</v>
+        <v>2424.883513345701</v>
       </c>
       <c r="D5" t="inlineStr"/>
     </row>
@@ -529,7 +529,7 @@
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>126.8499407842672</v>
+        <v>126.8499407842673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>